<commit_message>
Add RAG System for aromatherapy assistant
LangGraph-based RAG system that combines essential oils and herbal recommendations:
- Uses HuggingFace multilingual embeddings (Czech/Slovak support)
- 50/50 retrieval split between oils and herbs
- Professional aromatherapist persona
- Includes comprehensive documentation and setup instructions

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/2-Dataset/2-1-Raw_data/Fleurdin/EO_prehled oleju_30oils_updated.csv.xlsx
+++ b/2-Dataset/2-1-Raw_data/Fleurdin/EO_prehled oleju_30oils_updated.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Fleurdin_AI\Raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atlas/Projects/Fleurdin_AI/2-Dataset/2-1-Raw_data/Fleurdin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6E6679A2-4E91-4BB0-991B-6EDADE90F7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59567339-DB60-A245-AF08-1AD30629EE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D083F1BA-A11F-4D59-8472-9AFB43EF496B}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="23260" windowHeight="17140" xr2:uid="{D083F1BA-A11F-4D59-8472-9AFB43EF496B}"/>
   </bookViews>
   <sheets>
     <sheet name="EO_prehled oleju_raw data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="155">
   <si>
     <t>Esenciální oleje přehled</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Oregano - Dobromysl obecná</t>
-  </si>
-  <si>
-    <t>Doplnit</t>
   </si>
   <si>
     <t>Petitgrain</t>
@@ -722,12 +719,55 @@
   <si>
     <t>PSYCHIKA / EMOCE: Koriandr je olejem rovnováhy a uvolnění — propojuje tělo s myslí, odplavuje stres i toxiny a obnovuje přirozenou životní sílu. Přináší jemné povzbuzení a smyslnou harmonii. Povzbuzuje smysly, Pomáhá při emočním vyčerpání, Přináší rovnováhu mezi tělem a myslí, Posiluje sebedůvěru a vnitřní klid</t>
   </si>
+  <si>
+    <t>Není údaj</t>
+  </si>
+  <si>
+    <t>Frangipani</t>
+  </si>
+  <si>
+    <t>Plumeria alba</t>
+  </si>
+  <si>
+    <t>OBECNÉ: Protizánětlivý, Antioxidant, Sedativum
+KŮŽE: Hydratuje pokožku, Uvolňuje ucpané póry, Pomáhá při skvrnách, svědění a jizvách, Ulevuje při spáleninách od slunce, Pomáhá při suché a popraskané pokožce
+VLASY: Pomáhá při lupovitosti, Vyživuje a posiluje vlasy
+SVALY / ŠLACHY / KLOUBY: Ulevuje bolavým svalům, Pomáhá při artritidě, Ulevuje při bolestech zad
+BOLEST: Pomáhá při bolestech hlavy, Zmírňuje tinitus (hučení v uších)
+IMUNITA: Pomáhá při horečce
+NERVOVÝ SYSTÉM: Uklidňuje nervy, Pomáhá při nespavosti, Navozuje hluboký spánek a regeneraci
+SEXUALITA: Afrodisiakum, Zvyšuje libido</t>
+  </si>
+  <si>
+    <t>PSYCHIKA / EMOCE: Frangipani je olejem obnovy duše a smyslného klidu — symbolizuje znovuzrození, propojuje s hlubokým mírem a pomáhá navrátit lásku k sobě. Jemně otevírá srdce, uvolňuje napětí a přináší lehkost bytí. Pomáhá znovu nalézt radost, harmonii a duchovní sílu</t>
+  </si>
+  <si>
+    <t>Ho wood</t>
+  </si>
+  <si>
+    <t>Cinnamomum camphorum ct. Linalool</t>
+  </si>
+  <si>
+    <t>OBECNÉ: Antibakteriální, Analgetikum, Protiplísňový (na atletickou nohu), Protiparazitický, Sedativum
+KŮŽE: Čistí pleť, Hydratuje a stahuje póry, Omlazuje zralou pokožku, Pomáhá při akné a vráskách, Urychluje hojení a snižuje tvorbu jizev, Zmírňuje svědění a otoky, Má chladivý účinek na pokožku
+DÝCHÁNÍ: Pomáhá při nachlazení, chřipce a bronchitidě
+SVALY / ŠLACHY / KLOUBY: Pomáhá při bolestech svalů
+SRDCE / CÉVY: Zlepšuje krevní oběh
+HORMONÁLNÍ: Ulevuje při bolestivé menstruaci
+IMUNITA: Posiluje imunitní systém
+NERVOVÝ SYSTÉM: Uklidňuje při depresi, stresu, únavě a přepracování, Povzbuzuje i harmonizuje nervovou soustavu, Pomáhá při poruchách spánku, Uklidňuje tělo i mysl
+SEXUALITA: Afrodisiakum
+OSTATNÍ: Repelent</t>
+  </si>
+  <si>
+    <t>PSYCHIKA / EMOCE: Pomáhá rozbít nezdravé emocionální vzorce a závislosti na neuspokojivých situacích, Posiluje odvahu čelit změnám a skočit do neznáma, Uvolňuje napětí, přináší pocit klidu a sebedůvěry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +835,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -832,7 +878,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -851,7 +897,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -866,9 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -885,11 +927,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Nadpis 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Zvýraznění 3" xfId="2" builtinId="37"/>
+    <cellStyle name="Accent3" xfId="2" builtinId="37"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -905,7 +956,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1225,705 +1276,741 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32:XFD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.21875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="80.6640625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="50.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="80.6640625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="50.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="7.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="7.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="G3" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="288" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="224" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>20</v>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="335" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>9</v>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="316.8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="350" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>45</v>
+        <v>20</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" ht="345.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="365" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="7">
         <v>320</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>47</v>
+      <c r="F8" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="320" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>30</v>
+      <c r="E9" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="288" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="320" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="7">
         <v>96</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>87</v>
+      <c r="F10" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="350" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" ht="380" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>9</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="19">
+        <v>181</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" ht="288" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>11</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="E14" s="5">
         <v>580</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" ht="320" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>12</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" ht="320" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>13</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" ht="365" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="E17" s="5">
         <v>147</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="320" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>15</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="E18" s="5">
         <v>134</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="365" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>16</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="E19" s="5">
         <v>118</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" ht="288" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>17</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="360" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" ht="365" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="E21" s="5">
         <v>98</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="189" customHeight="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="189" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>19</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>98</v>
+      <c r="B22" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="E22" s="5">
         <v>120</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="360" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="380" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>20</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="E23" s="5">
         <v>78</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="331.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="350" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>21</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="E24" s="5">
         <v>102</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:7" ht="335" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>22</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="E25" s="5">
         <v>84</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:7" ht="380" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>23</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E26" s="5">
         <v>105</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="374.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:7" ht="395" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>24</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="E27" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="5">
-        <v>118</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:7" ht="380" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>25</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="E28" s="5">
         <v>52</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:7" ht="335" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>26</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="E29" s="5">
         <v>102</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:7" ht="304" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>27</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="E30" s="5">
         <v>105</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:7" ht="335" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>28</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="E31" s="5">
         <v>98</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:7" ht="256" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="335" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>30</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>